<commit_message>
updated operable test cases
</commit_message>
<xml_diff>
--- a/Distinguishable/WCAG_1.4.1_UseOfColor_Narayanan_Palani_TestCase_v1.xlsx
+++ b/Distinguishable/WCAG_1.4.1_UseOfColor_Narayanan_Palani_TestCase_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Udemy_Supreme_Quality\13 Write Accessibility Testing-Test Cases\GithubRepo\webAccessibilityTestCases\Distinguishable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A66312-D064-4077-927A-1C4DC01B17B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452BBA37-DE05-421C-8802-2E6060642321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20730" yWindow="525" windowWidth="15375" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Test Case Worksheet</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>WCAG_1.4.1_UseOfColor</t>
+  </si>
+  <si>
+    <t>Level Classification</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,24 +356,38 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,13 +757,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="4"/>
       <c r="H1" s="1"/>
     </row>
@@ -806,7 +823,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="8" t="str">
@@ -889,7 +906,9 @@
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
@@ -929,87 +948,87 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:11" s="26" customFormat="1" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="9" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" s="26" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="9" t="s">
+      <c r="G15" s="27"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" s="26" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="9" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+    </row>
+    <row r="17" spans="1:11" s="26" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>